<commit_message>
Updating the PSSdb list of projects
</commit_message>
<xml_diff>
--- a/raw/project_FlowCam_standardizer.xlsx
+++ b/raw/project_FlowCam_standardizer.xlsx
@@ -1127,20 +1127,20 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Variables</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Variable_types</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
@@ -1946,6 +1946,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>